<commit_message>
add multiple buy and sell swaps and add liquidity test
</commit_message>
<xml_diff>
--- a/contracts/amm_pair/ShadeSwapCalculation (version 1).xlsb.xlsx
+++ b/contracts/amm_pair/ShadeSwapCalculation (version 1).xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Polarity\shadeswap\contracts\amm_pair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535256BC-C1FE-4A4C-BAA4-DD8A40BC382D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CC6F59-37DA-4435-9C52-927DFE037283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
   </bookViews>
   <sheets>
     <sheet name="CalculationAmountAndPrice" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Snip 20 - SSRT</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Deducted Offer Amount</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49975B13-9A74-4599-A051-59B5C47586E4}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +612,7 @@
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -649,8 +652,11 @@
       <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10000000000</v>
       </c>
@@ -694,8 +700,12 @@
         <f xml:space="preserve"> INT((B2 *L2) / (A2 + L2))</f>
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <f xml:space="preserve"> M2/E2</f>
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2 +L2+H2</f>
         <v>10000000098</v>
@@ -741,8 +751,12 @@
         <f xml:space="preserve"> INT((B3 *L3) / (A3 + L3))</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <f xml:space="preserve"> M3/E3</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3 +L3+H3</f>
         <v>10000000147</v>
@@ -788,15 +802,19 @@
         <f xml:space="preserve"> INT((B4 *L4) / (A4 + L4))</f>
         <v>2249</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <f>(M4/E4) /1</f>
+        <v>0.89959999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>A4 +L4+H4</f>
-        <v>10000002597</v>
+        <f>A4 -M4</f>
+        <v>9999997898</v>
       </c>
       <c r="B5">
-        <f>B4-M4</f>
-        <v>9999997618</v>
+        <f>B4 +M4+H4</f>
+        <v>10000002316</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -835,15 +853,19 @@
         <f xml:space="preserve"> INT((B5 *L5) / (A5 + L5))</f>
         <v>32849</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <f>(M5/E5) /1</f>
+        <v>0.89997260273972601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>A5 +L5+H5</f>
-        <v>10000038367</v>
+        <f>A5 -M5</f>
+        <v>9999965049</v>
       </c>
       <c r="B6">
-        <f>B5-M5</f>
-        <v>9999964769</v>
+        <f>B5 + L5+H5</f>
+        <v>10000038086</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -880,17 +902,21 @@
       </c>
       <c r="M6">
         <f xml:space="preserve"> INT((B6 *L6) / (A6 + L6))</f>
-        <v>22499</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22500</v>
+      </c>
+      <c r="N6">
+        <f>M6/E6</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6 +L6+H6</f>
-        <v>10000062867</v>
+        <v>9999989549</v>
       </c>
       <c r="B7">
         <f>B6-M6</f>
-        <v>9999942270</v>
+        <v>10000015586</v>
       </c>
     </row>
   </sheetData>
@@ -903,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5474B69E-2599-48EB-8BEB-3B4FE80E24F9}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1220,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>